<commit_message>
Git fix timeout value in result_30m to be 1800
- Also fix performance plots
</commit_message>
<xml_diff>
--- a/performance/30m_results.xlsx
+++ b/performance/30m_results.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hahemthomas/Documents/Git/eduSAT-BVA/performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60967087-4946-AD42-A556-28FD67395D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0728E008-9306-3D43-9277-B1D4F6B507A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{13161F87-C3E4-4025-A621-1889FC01A28C}"/>
   </bookViews>
   <sheets>
     <sheet name="tmp" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tmp!$H$21:$H$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1738,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E5D71E-678E-4FB4-A1B0-A3485FC53E71}">
   <dimension ref="A1:L253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="G219" workbookViewId="0">
+      <selection activeCell="I231" sqref="I231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1794,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1822,7 +1825,7 @@
       </c>
       <c r="L2" s="1">
         <f t="shared" ref="L2:L65" si="0">C2/E2</f>
-        <v>6630.5180644781049</v>
+        <v>3315.2590322390524</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1833,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1861,7 +1864,7 @@
       </c>
       <c r="L3" s="1">
         <f t="shared" si="0"/>
-        <v>2547.2659345635684</v>
+        <v>1273.6329672817842</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1911,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1939,7 +1942,7 @@
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>107.93081634672174</v>
+        <v>53.965408173360871</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1950,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -1978,7 +1981,7 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
-        <v>106.95409589623075</v>
+        <v>53.477047948115377</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1989,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -2017,7 +2020,7 @@
       </c>
       <c r="L7" s="1">
         <f t="shared" si="0"/>
-        <v>42.269744373720904</v>
+        <v>21.134872186860452</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2028,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -2056,7 +2059,7 @@
       </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
-        <v>22.838002436053593</v>
+        <v>11.419001218026796</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2106,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -2134,7 +2137,7 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>3.5028996224652627</v>
+        <v>1.7514498112326313</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2184,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -2212,7 +2215,7 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="0"/>
-        <v>2.6496695273283968</v>
+        <v>1.3248347636641984</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -2301,13 +2304,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F15" s="1">
         <v>32837</v>
@@ -2334,13 +2337,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F16" s="1">
         <v>301</v>
@@ -2367,13 +2370,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F17" s="1">
         <v>80457</v>
@@ -2400,13 +2403,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F18" s="1">
         <v>12502</v>
@@ -2433,13 +2436,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F19" s="1">
         <v>45832</v>
@@ -2466,13 +2469,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F20" s="1">
         <v>4705</v>
@@ -2499,13 +2502,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F21" s="1">
         <v>1287</v>
@@ -2532,13 +2535,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F22" s="1">
         <v>941</v>
@@ -2565,13 +2568,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F23" s="1">
         <v>3913</v>
@@ -2598,13 +2601,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F24" s="1">
         <v>2</v>
@@ -2631,13 +2634,13 @@
         <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F25" s="1">
         <v>27930</v>
@@ -2664,13 +2667,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F26" s="1">
         <v>2014</v>
@@ -2697,13 +2700,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F27" s="1">
         <v>51</v>
@@ -2730,13 +2733,13 @@
         <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
       </c>
       <c r="E28" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F28" s="1">
         <v>45690</v>
@@ -2763,13 +2766,13 @@
         <v>1</v>
       </c>
       <c r="C29" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F29" s="1">
         <v>2014</v>
@@ -2796,13 +2799,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F30" s="1">
         <v>54</v>
@@ -2829,13 +2832,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F31" s="1">
         <v>11396</v>
@@ -2862,13 +2865,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F32" s="1">
         <v>4650</v>
@@ -2895,13 +2898,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F33" s="1">
         <v>29196</v>
@@ -2928,13 +2931,13 @@
         <v>1</v>
       </c>
       <c r="C34" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
       <c r="E34" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F34" s="1">
         <v>44821</v>
@@ -2961,13 +2964,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F35" s="1">
         <v>11981</v>
@@ -2994,13 +2997,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F36" s="1">
         <v>2343</v>
@@ -3027,13 +3030,13 @@
         <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
       </c>
       <c r="E37" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F37" s="1">
         <v>32692</v>
@@ -3060,13 +3063,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F38" s="1">
         <v>11</v>
@@ -3093,13 +3096,13 @@
         <v>1</v>
       </c>
       <c r="C39" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
       <c r="E39" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F39" s="1">
         <v>26958</v>
@@ -3126,13 +3129,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F40" s="1">
         <v>236</v>
@@ -3159,13 +3162,13 @@
         <v>1</v>
       </c>
       <c r="C41" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
       </c>
       <c r="E41" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F41" s="1">
         <v>1713</v>
@@ -3192,13 +3195,13 @@
         <v>1</v>
       </c>
       <c r="C42" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
       </c>
       <c r="E42" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F42" s="1">
         <v>566</v>
@@ -3225,13 +3228,13 @@
         <v>1</v>
       </c>
       <c r="C43" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F43" s="1">
         <v>1966</v>
@@ -3258,13 +3261,13 @@
         <v>1</v>
       </c>
       <c r="C44" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F44" s="1">
         <v>1026</v>
@@ -3291,13 +3294,13 @@
         <v>1</v>
       </c>
       <c r="C45" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
       </c>
       <c r="E45" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F45" s="1">
         <v>265</v>
@@ -3324,13 +3327,13 @@
         <v>1</v>
       </c>
       <c r="C46" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
       </c>
       <c r="E46" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F46" s="1">
         <v>69</v>
@@ -3357,13 +3360,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="E47" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F47" s="1">
         <v>24</v>
@@ -3390,13 +3393,13 @@
         <v>1</v>
       </c>
       <c r="C48" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F48" s="1">
         <v>6705</v>
@@ -3423,13 +3426,13 @@
         <v>1</v>
       </c>
       <c r="C49" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F49" s="1">
         <v>167767</v>
@@ -3456,13 +3459,13 @@
         <v>1</v>
       </c>
       <c r="C50" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F50" s="1">
         <v>32842</v>
@@ -3489,13 +3492,13 @@
         <v>1</v>
       </c>
       <c r="C51" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
       <c r="E51" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F51" s="1">
         <v>27693</v>
@@ -3522,13 +3525,13 @@
         <v>1</v>
       </c>
       <c r="C52" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="E52" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F52" s="1">
         <v>4694</v>
@@ -3555,13 +3558,13 @@
         <v>1</v>
       </c>
       <c r="C53" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D53" s="1">
         <v>1</v>
       </c>
       <c r="E53" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F53" s="1">
         <v>48416</v>
@@ -3588,13 +3591,13 @@
         <v>1</v>
       </c>
       <c r="C54" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="E54" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F54" s="1">
         <v>6109</v>
@@ -3621,13 +3624,13 @@
         <v>1</v>
       </c>
       <c r="C55" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="E55" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F55" s="1">
         <v>52</v>
@@ -3654,13 +3657,13 @@
         <v>1</v>
       </c>
       <c r="C56" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="E56" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F56" s="1">
         <v>7440</v>
@@ -3687,13 +3690,13 @@
         <v>1</v>
       </c>
       <c r="C57" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="E57" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F57" s="1">
         <v>881</v>
@@ -3720,13 +3723,13 @@
         <v>1</v>
       </c>
       <c r="C58" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F58" s="1">
         <v>45366</v>
@@ -3753,13 +3756,13 @@
         <v>1</v>
       </c>
       <c r="C59" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="E59" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F59" s="1">
         <v>11340</v>
@@ -3786,13 +3789,13 @@
         <v>1</v>
       </c>
       <c r="C60" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="E60" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F60" s="1">
         <v>4088</v>
@@ -3819,13 +3822,13 @@
         <v>1</v>
       </c>
       <c r="C61" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
       </c>
       <c r="E61" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F61" s="1">
         <v>31911</v>
@@ -3852,13 +3855,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D62" s="1">
         <v>1</v>
       </c>
       <c r="E62" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F62" s="1">
         <v>33677</v>
@@ -3885,13 +3888,13 @@
         <v>1</v>
       </c>
       <c r="C63" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D63" s="1">
         <v>1</v>
       </c>
       <c r="E63" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F63" s="1">
         <v>10541</v>
@@ -3918,13 +3921,13 @@
         <v>1</v>
       </c>
       <c r="C64" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D64" s="1">
         <v>1</v>
       </c>
       <c r="E64" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F64" s="1">
         <v>17082</v>
@@ -3951,13 +3954,13 @@
         <v>1</v>
       </c>
       <c r="C65" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D65" s="1">
         <v>1</v>
       </c>
       <c r="E65" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F65" s="1">
         <v>52175</v>
@@ -3984,13 +3987,13 @@
         <v>1</v>
       </c>
       <c r="C66" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D66" s="1">
         <v>1</v>
       </c>
       <c r="E66" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F66" s="1">
         <v>17082</v>
@@ -4017,13 +4020,13 @@
         <v>1</v>
       </c>
       <c r="C67" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D67" s="1">
         <v>1</v>
       </c>
       <c r="E67" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F67" s="1">
         <v>4075</v>
@@ -4050,13 +4053,13 @@
         <v>1</v>
       </c>
       <c r="C68" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="E68" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F68" s="1">
         <v>1375</v>
@@ -4083,13 +4086,13 @@
         <v>1</v>
       </c>
       <c r="C69" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="E69" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F69" s="1">
         <v>27510</v>
@@ -4116,13 +4119,13 @@
         <v>1</v>
       </c>
       <c r="C70" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
       <c r="E70" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F70" s="1">
         <v>98111</v>
@@ -4149,13 +4152,13 @@
         <v>1</v>
       </c>
       <c r="C71" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
       <c r="E71" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F71" s="1">
         <v>45199</v>
@@ -4182,13 +4185,13 @@
         <v>1</v>
       </c>
       <c r="C72" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D72" s="1">
         <v>1</v>
       </c>
       <c r="E72" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F72" s="1">
         <v>3913</v>
@@ -4215,13 +4218,13 @@
         <v>1</v>
       </c>
       <c r="C73" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D73" s="1">
         <v>1</v>
       </c>
       <c r="E73" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F73" s="1">
         <v>768</v>
@@ -4248,13 +4251,13 @@
         <v>1</v>
       </c>
       <c r="C74" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D74" s="1">
         <v>1</v>
       </c>
       <c r="E74" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F74" s="1">
         <v>50</v>
@@ -4281,13 +4284,13 @@
         <v>1</v>
       </c>
       <c r="C75" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D75" s="1">
         <v>1</v>
       </c>
       <c r="E75" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F75" s="1">
         <v>46298</v>
@@ -4314,13 +4317,13 @@
         <v>1</v>
       </c>
       <c r="C76" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="E76" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F76" s="1">
         <v>57164</v>
@@ -4347,13 +4350,13 @@
         <v>1</v>
       </c>
       <c r="C77" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="E77" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F77" s="1">
         <v>310</v>
@@ -4380,13 +4383,13 @@
         <v>1</v>
       </c>
       <c r="C78" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
       </c>
       <c r="E78" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F78" s="1">
         <v>32449</v>
@@ -4413,13 +4416,13 @@
         <v>1</v>
       </c>
       <c r="C79" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
       </c>
       <c r="E79" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F79" s="1">
         <v>38425</v>
@@ -4446,13 +4449,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D80" s="1">
         <v>1</v>
       </c>
       <c r="E80" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F80" s="1">
         <v>32734</v>
@@ -4479,13 +4482,13 @@
         <v>1</v>
       </c>
       <c r="C81" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D81" s="1">
         <v>1</v>
       </c>
       <c r="E81" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F81" s="1">
         <v>941</v>
@@ -4512,13 +4515,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D82" s="1">
         <v>1</v>
       </c>
       <c r="E82" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F82" s="1">
         <v>250</v>
@@ -4545,13 +4548,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D83" s="1">
         <v>1</v>
       </c>
       <c r="E83" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F83" s="1">
         <v>55497</v>
@@ -4578,13 +4581,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="E84" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F84" s="1">
         <v>49124</v>
@@ -4611,13 +4614,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
       </c>
       <c r="E85" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F85" s="1">
         <v>23</v>
@@ -4644,13 +4647,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
       </c>
       <c r="E86" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F86" s="1">
         <v>3913</v>
@@ -4677,13 +4680,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
       <c r="E87" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F87" s="1">
         <v>32500</v>
@@ -4710,13 +4713,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D88" s="1">
         <v>1</v>
       </c>
       <c r="E88" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F88" s="1">
         <v>54939</v>
@@ -4743,13 +4746,13 @@
         <v>1</v>
       </c>
       <c r="C89" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D89" s="1">
         <v>1</v>
       </c>
       <c r="E89" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F89" s="1">
         <v>30178</v>
@@ -4776,13 +4779,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D90" s="1">
         <v>1</v>
       </c>
       <c r="E90" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F90" s="1">
         <v>57016</v>
@@ -4809,13 +4812,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D91" s="1">
         <v>1</v>
       </c>
       <c r="E91" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F91" s="1">
         <v>312</v>
@@ -4842,13 +4845,13 @@
         <v>1</v>
       </c>
       <c r="C92" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D92" s="1">
         <v>1</v>
       </c>
       <c r="E92" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F92" s="1">
         <v>49155</v>
@@ -4875,13 +4878,13 @@
         <v>1</v>
       </c>
       <c r="C93" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D93" s="1">
         <v>1</v>
       </c>
       <c r="E93" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F93" s="1">
         <v>2712</v>
@@ -4908,13 +4911,13 @@
         <v>1</v>
       </c>
       <c r="C94" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D94" s="1">
         <v>1</v>
       </c>
       <c r="E94" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F94" s="1">
         <v>6109</v>
@@ -4941,13 +4944,13 @@
         <v>1</v>
       </c>
       <c r="C95" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D95" s="1">
         <v>1</v>
       </c>
       <c r="E95" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F95" s="1">
         <v>32465</v>
@@ -4974,13 +4977,13 @@
         <v>1</v>
       </c>
       <c r="C96" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D96" s="1">
         <v>1</v>
       </c>
       <c r="E96" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F96" s="1">
         <v>42881</v>
@@ -5007,13 +5010,13 @@
         <v>1</v>
       </c>
       <c r="C97" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D97" s="1">
         <v>1</v>
       </c>
       <c r="E97" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F97" s="1">
         <v>123801</v>
@@ -5040,13 +5043,13 @@
         <v>1</v>
       </c>
       <c r="C98" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D98" s="1">
         <v>1</v>
       </c>
       <c r="E98" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F98" s="1">
         <v>32434</v>
@@ -5073,13 +5076,13 @@
         <v>1</v>
       </c>
       <c r="C99" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D99" s="1">
         <v>1</v>
       </c>
       <c r="E99" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F99" s="1">
         <v>70</v>
@@ -5106,13 +5109,13 @@
         <v>1</v>
       </c>
       <c r="C100" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D100" s="1">
         <v>1</v>
       </c>
       <c r="E100" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F100" s="1">
         <v>25</v>
@@ -5139,13 +5142,13 @@
         <v>1</v>
       </c>
       <c r="C101" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D101" s="1">
         <v>1</v>
       </c>
       <c r="E101" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F101" s="1">
         <v>120</v>
@@ -5172,13 +5175,13 @@
         <v>1</v>
       </c>
       <c r="C102" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D102" s="1">
         <v>1</v>
       </c>
       <c r="E102" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F102" s="1">
         <v>43221</v>
@@ -5205,13 +5208,13 @@
         <v>1</v>
       </c>
       <c r="C103" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D103" s="1">
         <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F103" s="1">
         <v>3913</v>
@@ -5238,13 +5241,13 @@
         <v>1</v>
       </c>
       <c r="C104" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
       <c r="E104" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F104" s="1">
         <v>869</v>
@@ -5271,13 +5274,13 @@
         <v>1</v>
       </c>
       <c r="C105" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D105" s="1">
         <v>1</v>
       </c>
       <c r="E105" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F105" s="1">
         <v>3913</v>
@@ -5304,13 +5307,13 @@
         <v>1</v>
       </c>
       <c r="C106" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D106" s="1">
         <v>1</v>
       </c>
       <c r="E106" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F106" s="1">
         <v>16043</v>
@@ -5337,13 +5340,13 @@
         <v>1</v>
       </c>
       <c r="C107" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D107" s="1">
         <v>1</v>
       </c>
       <c r="E107" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F107" s="1">
         <v>12543</v>
@@ -5370,13 +5373,13 @@
         <v>1</v>
       </c>
       <c r="C108" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D108" s="1">
         <v>1</v>
       </c>
       <c r="E108" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F108" s="1">
         <v>3913</v>
@@ -5403,13 +5406,13 @@
         <v>1</v>
       </c>
       <c r="C109" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D109" s="1">
         <v>1</v>
       </c>
       <c r="E109" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F109" s="1">
         <v>1147</v>
@@ -5436,13 +5439,13 @@
         <v>1</v>
       </c>
       <c r="C110" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D110" s="1">
         <v>1</v>
       </c>
       <c r="E110" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F110" s="1">
         <v>52</v>
@@ -5469,13 +5472,13 @@
         <v>1</v>
       </c>
       <c r="C111" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D111" s="1">
         <v>1</v>
       </c>
       <c r="E111" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F111" s="1">
         <v>25643</v>
@@ -5502,13 +5505,13 @@
         <v>1</v>
       </c>
       <c r="C112" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D112" s="1">
         <v>1</v>
       </c>
       <c r="E112" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F112" s="1">
         <v>30246</v>
@@ -5535,13 +5538,13 @@
         <v>1</v>
       </c>
       <c r="C113" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D113" s="1">
         <v>1</v>
       </c>
       <c r="E113" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F113" s="1">
         <v>486981</v>
@@ -5568,13 +5571,13 @@
         <v>1</v>
       </c>
       <c r="C114" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D114" s="1">
         <v>1</v>
       </c>
       <c r="E114" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F114" s="1">
         <v>4930</v>
@@ -5601,13 +5604,13 @@
         <v>1</v>
       </c>
       <c r="C115" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D115" s="1">
         <v>1</v>
       </c>
       <c r="E115" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F115" s="1">
         <v>704</v>
@@ -5634,13 +5637,13 @@
         <v>1</v>
       </c>
       <c r="C116" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D116" s="1">
         <v>1</v>
       </c>
       <c r="E116" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F116" s="1">
         <v>1976</v>
@@ -5667,13 +5670,13 @@
         <v>1</v>
       </c>
       <c r="C117" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D117" s="1">
         <v>1</v>
       </c>
       <c r="E117" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F117" s="1">
         <v>42911</v>
@@ -5700,13 +5703,13 @@
         <v>1</v>
       </c>
       <c r="C118" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D118" s="1">
         <v>1</v>
       </c>
       <c r="E118" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F118" s="1">
         <v>3108</v>
@@ -5733,13 +5736,13 @@
         <v>1</v>
       </c>
       <c r="C119" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D119" s="1">
         <v>1</v>
       </c>
       <c r="E119" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F119" s="1">
         <v>53</v>
@@ -5766,13 +5769,13 @@
         <v>1</v>
       </c>
       <c r="C120" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D120" s="1">
         <v>1</v>
       </c>
       <c r="E120" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F120" s="1">
         <v>52495</v>
@@ -5799,13 +5802,13 @@
         <v>1</v>
       </c>
       <c r="C121" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D121" s="1">
         <v>1</v>
       </c>
       <c r="E121" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F121" s="1">
         <v>36346</v>
@@ -5832,13 +5835,13 @@
         <v>1</v>
       </c>
       <c r="C122" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D122" s="1">
         <v>1</v>
       </c>
       <c r="E122" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F122" s="1">
         <v>33125</v>
@@ -5865,13 +5868,13 @@
         <v>1</v>
       </c>
       <c r="C123" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D123" s="1">
         <v>1</v>
       </c>
       <c r="E123" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F123" s="1">
         <v>4705</v>
@@ -5898,13 +5901,13 @@
         <v>1</v>
       </c>
       <c r="C124" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D124" s="1">
         <v>1</v>
       </c>
       <c r="E124" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F124" s="1">
         <v>5152</v>
@@ -5931,13 +5934,13 @@
         <v>1</v>
       </c>
       <c r="C125" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D125" s="1">
         <v>1</v>
       </c>
       <c r="E125" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F125" s="1">
         <v>557</v>
@@ -5964,13 +5967,13 @@
         <v>1</v>
       </c>
       <c r="C126" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D126" s="1">
         <v>1</v>
       </c>
       <c r="E126" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F126" s="1">
         <v>3913</v>
@@ -5997,13 +6000,13 @@
         <v>1</v>
       </c>
       <c r="C127" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D127" s="1">
         <v>1</v>
       </c>
       <c r="E127" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F127" s="1">
         <v>38932</v>
@@ -6030,13 +6033,13 @@
         <v>1</v>
       </c>
       <c r="C128" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D128" s="1">
         <v>1</v>
       </c>
       <c r="E128" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F128" s="1">
         <v>236</v>
@@ -6063,13 +6066,13 @@
         <v>1</v>
       </c>
       <c r="C129" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D129" s="1">
         <v>1</v>
       </c>
       <c r="E129" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F129" s="1">
         <v>99180</v>
@@ -6096,13 +6099,13 @@
         <v>1</v>
       </c>
       <c r="C130" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D130" s="1">
         <v>1</v>
       </c>
       <c r="E130" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F130" s="1">
         <v>2014</v>
@@ -6129,13 +6132,13 @@
         <v>1</v>
       </c>
       <c r="C131" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D131" s="1">
         <v>1</v>
       </c>
       <c r="E131" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F131" s="1">
         <v>2014</v>
@@ -6162,13 +6165,13 @@
         <v>1</v>
       </c>
       <c r="C132" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D132" s="1">
         <v>1</v>
       </c>
       <c r="E132" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F132" s="1">
         <v>50</v>
@@ -6195,13 +6198,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D133" s="1">
         <v>1</v>
       </c>
       <c r="E133" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F133" s="1">
         <v>17504</v>
@@ -6228,13 +6231,13 @@
         <v>1</v>
       </c>
       <c r="C134" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D134" s="1">
         <v>1</v>
       </c>
       <c r="E134" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F134" s="1">
         <v>1979</v>
@@ -6261,13 +6264,13 @@
         <v>1</v>
       </c>
       <c r="C135" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D135" s="1">
         <v>1</v>
       </c>
       <c r="E135" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F135" s="1">
         <v>2014</v>
@@ -6294,13 +6297,13 @@
         <v>1</v>
       </c>
       <c r="C136" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D136" s="1">
         <v>1</v>
       </c>
       <c r="E136" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F136" s="1">
         <v>51403</v>
@@ -6327,13 +6330,13 @@
         <v>1</v>
       </c>
       <c r="C137" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D137" s="1">
         <v>1</v>
       </c>
       <c r="E137" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F137" s="1">
         <v>54</v>
@@ -6360,13 +6363,13 @@
         <v>1</v>
       </c>
       <c r="C138" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D138" s="1">
         <v>1</v>
       </c>
       <c r="E138" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F138" s="1">
         <v>56996</v>
@@ -6393,13 +6396,13 @@
         <v>1</v>
       </c>
       <c r="C139" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D139" s="1">
         <v>1</v>
       </c>
       <c r="E139" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F139" s="1">
         <v>881</v>
@@ -6426,13 +6429,13 @@
         <v>1</v>
       </c>
       <c r="C140" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D140" s="1">
         <v>1</v>
       </c>
       <c r="E140" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F140" s="1">
         <v>27999</v>
@@ -6459,13 +6462,13 @@
         <v>1</v>
       </c>
       <c r="C141" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D141" s="1">
         <v>1</v>
       </c>
       <c r="E141" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F141" s="1">
         <v>52800</v>
@@ -6492,13 +6495,13 @@
         <v>1</v>
       </c>
       <c r="C142" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D142" s="1">
         <v>1</v>
       </c>
       <c r="E142" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F142" s="1">
         <v>53</v>
@@ -6525,13 +6528,13 @@
         <v>1</v>
       </c>
       <c r="C143" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D143" s="1">
         <v>1</v>
       </c>
       <c r="E143" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F143" s="1">
         <v>32787</v>
@@ -6558,13 +6561,13 @@
         <v>1</v>
       </c>
       <c r="C144" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D144" s="1">
         <v>1</v>
       </c>
       <c r="E144" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F144" s="1">
         <v>686</v>
@@ -6591,13 +6594,13 @@
         <v>1</v>
       </c>
       <c r="C145" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D145" s="1">
         <v>1</v>
       </c>
       <c r="E145" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F145" s="1">
         <v>3339</v>
@@ -6624,13 +6627,13 @@
         <v>1</v>
       </c>
       <c r="C146" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D146" s="1">
         <v>1</v>
       </c>
       <c r="E146" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F146" s="1">
         <v>4527</v>
@@ -6657,13 +6660,13 @@
         <v>1</v>
       </c>
       <c r="C147" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D147" s="1">
         <v>1</v>
       </c>
       <c r="E147" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F147" s="1">
         <v>96160</v>
@@ -6690,13 +6693,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D148" s="1">
         <v>1</v>
       </c>
       <c r="E148" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F148" s="1">
         <v>32632</v>
@@ -6723,13 +6726,13 @@
         <v>1</v>
       </c>
       <c r="C149" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D149" s="1">
         <v>1</v>
       </c>
       <c r="E149" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F149" s="1">
         <v>3913</v>
@@ -6756,13 +6759,13 @@
         <v>1</v>
       </c>
       <c r="C150" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D150" s="1">
         <v>1</v>
       </c>
       <c r="E150" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F150" s="1">
         <v>32580</v>
@@ -6789,13 +6792,13 @@
         <v>1</v>
       </c>
       <c r="C151" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D151" s="1">
         <v>1</v>
       </c>
       <c r="E151" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F151" s="1">
         <v>31950</v>
@@ -6822,13 +6825,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D152" s="1">
         <v>1</v>
       </c>
       <c r="E152" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F152" s="1">
         <v>36346</v>
@@ -6855,13 +6858,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D153" s="1">
         <v>1</v>
       </c>
       <c r="E153" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F153" s="1">
         <v>22</v>
@@ -6888,13 +6891,13 @@
         <v>1</v>
       </c>
       <c r="C154" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D154" s="1">
         <v>1</v>
       </c>
       <c r="E154" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F154" s="1">
         <v>60</v>
@@ -6921,13 +6924,13 @@
         <v>1</v>
       </c>
       <c r="C155" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D155" s="1">
         <v>1</v>
       </c>
       <c r="E155" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F155" s="1">
         <v>42095</v>
@@ -6954,13 +6957,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D156" s="1">
         <v>1</v>
       </c>
       <c r="E156" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F156" s="1">
         <v>4705</v>
@@ -6987,13 +6990,13 @@
         <v>1</v>
       </c>
       <c r="C157" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D157" s="1">
         <v>1</v>
       </c>
       <c r="E157" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F157" s="1">
         <v>1404</v>
@@ -7020,13 +7023,13 @@
         <v>1</v>
       </c>
       <c r="C158" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D158" s="1">
         <v>1</v>
       </c>
       <c r="E158" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F158" s="1">
         <v>3060</v>
@@ -7053,13 +7056,13 @@
         <v>1</v>
       </c>
       <c r="C159" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D159" s="1">
         <v>1</v>
       </c>
       <c r="E159" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F159" s="1">
         <v>880</v>
@@ -7086,13 +7089,13 @@
         <v>1</v>
       </c>
       <c r="C160" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D160" s="1">
         <v>1</v>
       </c>
       <c r="E160" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F160" s="1">
         <v>2410777</v>
@@ -7119,13 +7122,13 @@
         <v>1</v>
       </c>
       <c r="C161" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D161" s="1">
         <v>1</v>
       </c>
       <c r="E161" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F161" s="1">
         <v>39894</v>
@@ -7152,13 +7155,13 @@
         <v>1</v>
       </c>
       <c r="C162" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D162" s="1">
         <v>1</v>
       </c>
       <c r="E162" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F162" s="1">
         <v>41257</v>
@@ -7185,13 +7188,13 @@
         <v>1</v>
       </c>
       <c r="C163" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D163" s="1">
         <v>1</v>
       </c>
       <c r="E163" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F163" s="1">
         <v>50481</v>
@@ -7218,13 +7221,13 @@
         <v>1</v>
       </c>
       <c r="C164" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D164" s="1">
         <v>1</v>
       </c>
       <c r="E164" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F164" s="1">
         <v>10416</v>
@@ -7251,13 +7254,13 @@
         <v>1</v>
       </c>
       <c r="C165" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D165" s="1">
         <v>1</v>
       </c>
       <c r="E165" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F165" s="1">
         <v>6279</v>
@@ -7284,13 +7287,13 @@
         <v>1</v>
       </c>
       <c r="C166" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D166" s="1">
         <v>1</v>
       </c>
       <c r="E166" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F166" s="1">
         <v>32722</v>
@@ -7317,13 +7320,13 @@
         <v>1</v>
       </c>
       <c r="C167" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D167" s="1">
         <v>1</v>
       </c>
       <c r="E167" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F167" s="1">
         <v>49795</v>
@@ -7350,13 +7353,13 @@
         <v>1</v>
       </c>
       <c r="C168" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D168" s="1">
         <v>1</v>
       </c>
       <c r="E168" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F168" s="1">
         <v>2014</v>
@@ -7383,13 +7386,13 @@
         <v>1</v>
       </c>
       <c r="C169" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D169" s="1">
         <v>1</v>
       </c>
       <c r="E169" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F169" s="1">
         <v>1308</v>
@@ -7416,13 +7419,13 @@
         <v>1</v>
       </c>
       <c r="C170" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D170" s="1">
         <v>1</v>
       </c>
       <c r="E170" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F170" s="1">
         <v>1798</v>
@@ -7449,13 +7452,13 @@
         <v>1</v>
       </c>
       <c r="C171" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D171" s="1">
         <v>1</v>
       </c>
       <c r="E171" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F171" s="1">
         <v>96160</v>
@@ -7482,13 +7485,13 @@
         <v>1</v>
       </c>
       <c r="C172" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D172" s="1">
         <v>1</v>
       </c>
       <c r="E172" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F172" s="1">
         <v>140</v>
@@ -7515,13 +7518,13 @@
         <v>1</v>
       </c>
       <c r="C173" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D173" s="1">
         <v>1</v>
       </c>
       <c r="E173" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F173" s="1">
         <v>40497</v>
@@ -7548,13 +7551,13 @@
         <v>1</v>
       </c>
       <c r="C174" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D174" s="1">
         <v>1</v>
       </c>
       <c r="E174" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F174" s="1">
         <v>48</v>
@@ -7581,13 +7584,13 @@
         <v>1</v>
       </c>
       <c r="C175" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D175" s="1">
         <v>1</v>
       </c>
       <c r="E175" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F175" s="1">
         <v>1428</v>
@@ -7614,13 +7617,13 @@
         <v>1</v>
       </c>
       <c r="C176" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D176" s="1">
         <v>1</v>
       </c>
       <c r="E176" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F176" s="1">
         <v>19351</v>
@@ -7647,13 +7650,13 @@
         <v>1</v>
       </c>
       <c r="C177" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D177" s="1">
         <v>1</v>
       </c>
       <c r="E177" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F177" s="1">
         <v>33031</v>
@@ -7680,13 +7683,13 @@
         <v>1</v>
       </c>
       <c r="C178" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D178" s="1">
         <v>1</v>
       </c>
       <c r="E178" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F178" s="1">
         <v>2448</v>
@@ -7713,13 +7716,13 @@
         <v>1</v>
       </c>
       <c r="C179" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D179" s="1">
         <v>1</v>
       </c>
       <c r="E179" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F179" s="1">
         <v>5786</v>
@@ -7746,13 +7749,13 @@
         <v>1</v>
       </c>
       <c r="C180" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D180" s="1">
         <v>1</v>
       </c>
       <c r="E180" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F180" s="1">
         <v>36262</v>
@@ -7779,13 +7782,13 @@
         <v>1</v>
       </c>
       <c r="C181" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D181" s="1">
         <v>1</v>
       </c>
       <c r="E181" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F181" s="1">
         <v>20927</v>
@@ -7812,13 +7815,13 @@
         <v>1</v>
       </c>
       <c r="C182" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D182" s="1">
         <v>1</v>
       </c>
       <c r="E182" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F182" s="1">
         <v>126</v>
@@ -7845,13 +7848,13 @@
         <v>1</v>
       </c>
       <c r="C183" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D183" s="1">
         <v>1</v>
       </c>
       <c r="E183" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F183" s="1">
         <v>2014</v>
@@ -7878,13 +7881,13 @@
         <v>1</v>
       </c>
       <c r="C184" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D184" s="1">
         <v>1</v>
       </c>
       <c r="E184" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F184" s="1">
         <v>1118</v>
@@ -7911,13 +7914,13 @@
         <v>1</v>
       </c>
       <c r="C185" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D185" s="1">
         <v>1</v>
       </c>
       <c r="E185" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F185" s="1">
         <v>2291</v>
@@ -7944,13 +7947,13 @@
         <v>1</v>
       </c>
       <c r="C186" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D186" s="1">
         <v>1</v>
       </c>
       <c r="E186" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F186" s="1">
         <v>4803</v>
@@ -7977,13 +7980,13 @@
         <v>1</v>
       </c>
       <c r="C187" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D187" s="1">
         <v>1</v>
       </c>
       <c r="E187" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F187" s="1">
         <v>224842</v>
@@ -8010,13 +8013,13 @@
         <v>1</v>
       </c>
       <c r="C188" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D188" s="1">
         <v>1</v>
       </c>
       <c r="E188" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F188" s="1">
         <v>48505</v>
@@ -8043,13 +8046,13 @@
         <v>1</v>
       </c>
       <c r="C189" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D189" s="1">
         <v>1</v>
       </c>
       <c r="E189" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F189" s="1">
         <v>479</v>
@@ -8076,13 +8079,13 @@
         <v>1</v>
       </c>
       <c r="C190" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D190" s="1">
         <v>1</v>
       </c>
       <c r="E190" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F190" s="1">
         <v>49</v>
@@ -8109,13 +8112,13 @@
         <v>1</v>
       </c>
       <c r="C191" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D191" s="1">
         <v>1</v>
       </c>
       <c r="E191" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F191" s="1">
         <v>28424</v>
@@ -8142,13 +8145,13 @@
         <v>1</v>
       </c>
       <c r="C192" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D192" s="1">
         <v>1</v>
       </c>
       <c r="E192" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F192" s="1">
         <v>10582</v>
@@ -8175,13 +8178,13 @@
         <v>1</v>
       </c>
       <c r="C193" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D193" s="1">
         <v>1</v>
       </c>
       <c r="E193" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F193" s="1">
         <v>11</v>
@@ -8208,13 +8211,13 @@
         <v>1</v>
       </c>
       <c r="C194" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D194" s="1">
         <v>1</v>
       </c>
       <c r="E194" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F194" s="1">
         <v>54587</v>
@@ -8241,13 +8244,13 @@
         <v>1</v>
       </c>
       <c r="C195" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D195" s="1">
         <v>1</v>
       </c>
       <c r="E195" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F195" s="1">
         <v>390</v>
@@ -8274,13 +8277,13 @@
         <v>1</v>
       </c>
       <c r="C196" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D196" s="1">
         <v>1</v>
       </c>
       <c r="E196" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F196" s="1">
         <v>828</v>
@@ -8307,13 +8310,13 @@
         <v>1</v>
       </c>
       <c r="C197" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D197" s="1">
         <v>1</v>
       </c>
       <c r="E197" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F197" s="1">
         <v>62917</v>
@@ -8340,13 +8343,13 @@
         <v>1</v>
       </c>
       <c r="C198" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D198" s="1">
         <v>1</v>
       </c>
       <c r="E198" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F198" s="1">
         <v>33096</v>
@@ -8373,13 +8376,13 @@
         <v>1</v>
       </c>
       <c r="C199" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D199" s="1">
         <v>1</v>
       </c>
       <c r="E199" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F199" s="1">
         <v>43259</v>
@@ -8406,13 +8409,13 @@
         <v>1</v>
       </c>
       <c r="C200" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D200" s="1">
         <v>1</v>
       </c>
       <c r="E200" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F200" s="1">
         <v>3864</v>
@@ -8439,13 +8442,13 @@
         <v>1</v>
       </c>
       <c r="C201" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D201" s="1">
         <v>1</v>
       </c>
       <c r="E201" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F201" s="1">
         <v>4960</v>
@@ -8472,13 +8475,13 @@
         <v>1</v>
       </c>
       <c r="C202" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D202" s="1">
         <v>1</v>
       </c>
       <c r="E202" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="L202" s="1">
         <f t="shared" si="3"/>
@@ -8493,13 +8496,13 @@
         <v>1</v>
       </c>
       <c r="C203" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D203" s="1">
         <v>1</v>
       </c>
       <c r="E203" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F203" s="1">
         <v>2379</v>
@@ -8526,13 +8529,13 @@
         <v>1</v>
       </c>
       <c r="C204" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D204" s="1">
         <v>1</v>
       </c>
       <c r="E204" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F204" s="1">
         <v>55</v>
@@ -8559,13 +8562,13 @@
         <v>1</v>
       </c>
       <c r="C205" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D205" s="1">
         <v>1</v>
       </c>
       <c r="E205" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F205" s="1">
         <v>13299</v>
@@ -8592,13 +8595,13 @@
         <v>1</v>
       </c>
       <c r="C206" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D206" s="1">
         <v>1</v>
       </c>
       <c r="E206" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F206" s="1">
         <v>52</v>
@@ -8625,13 +8628,13 @@
         <v>1</v>
       </c>
       <c r="C207" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D207" s="1">
         <v>1</v>
       </c>
       <c r="E207" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F207" s="1">
         <v>4855</v>
@@ -8658,13 +8661,13 @@
         <v>1</v>
       </c>
       <c r="C208" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D208" s="1">
         <v>1</v>
       </c>
       <c r="E208" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F208" s="1">
         <v>268</v>
@@ -8691,13 +8694,13 @@
         <v>1</v>
       </c>
       <c r="C209" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D209" s="1">
         <v>1</v>
       </c>
       <c r="E209" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F209" s="1">
         <v>5879</v>
@@ -8724,13 +8727,13 @@
         <v>1</v>
       </c>
       <c r="C210" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D210" s="1">
         <v>1</v>
       </c>
       <c r="E210" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F210" s="1">
         <v>1417</v>
@@ -8757,13 +8760,13 @@
         <v>1</v>
       </c>
       <c r="C211" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D211" s="1">
         <v>1</v>
       </c>
       <c r="E211" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F211" s="1">
         <v>12948</v>
@@ -8790,13 +8793,13 @@
         <v>1</v>
       </c>
       <c r="C212" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D212" s="1">
         <v>1</v>
       </c>
       <c r="E212" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F212" s="1">
         <v>3750</v>
@@ -8823,13 +8826,13 @@
         <v>1</v>
       </c>
       <c r="C213" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D213" s="1">
         <v>1</v>
       </c>
       <c r="E213" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F213" s="1">
         <v>1530</v>
@@ -8856,13 +8859,13 @@
         <v>1</v>
       </c>
       <c r="C214" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="D214" s="1">
         <v>1</v>
       </c>
       <c r="E214" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F214" s="1">
         <v>33129</v>
@@ -9558,7 +9561,7 @@
         <v>1</v>
       </c>
       <c r="E232" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F232" s="1">
         <v>10277</v>
@@ -9574,7 +9577,7 @@
       </c>
       <c r="L232" s="1">
         <f t="shared" si="3"/>
-        <v>0.38398055555555555</v>
+        <v>0.76796111111111109</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
@@ -9669,7 +9672,7 @@
         <v>1</v>
       </c>
       <c r="E235" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F235" s="1">
         <v>30465</v>
@@ -9685,7 +9688,7 @@
       </c>
       <c r="L235" s="1">
         <f t="shared" si="3"/>
-        <v>0.28798888888888891</v>
+        <v>0.57597777777777781</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
@@ -9741,11 +9744,11 @@
         <v>1</v>
       </c>
       <c r="E237" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="L237" s="1">
         <f t="shared" si="3"/>
-        <v>0.25658722222222224</v>
+        <v>0.51317444444444449</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
@@ -9957,7 +9960,7 @@
         <v>1</v>
       </c>
       <c r="E243" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F243" s="1">
         <v>189</v>
@@ -9973,7 +9976,7 @@
       </c>
       <c r="L243" s="1">
         <f t="shared" si="3"/>
-        <v>0.18540972222222224</v>
+        <v>0.37081944444444448</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
@@ -10107,7 +10110,7 @@
         <v>1</v>
       </c>
       <c r="E247" s="1">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="F247" s="1">
         <v>3150</v>
@@ -10123,7 +10126,7 @@
       </c>
       <c r="L247" s="1">
         <f t="shared" si="3"/>
-        <v>0.13138555555555556</v>
+        <v>0.26277111111111112</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
@@ -10361,6 +10364,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H21:H22" xr:uid="{08E5D71E-678E-4FB4-A1B0-A3485FC53E71}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L253">
     <sortCondition descending="1" ref="L2:L253"/>
   </sortState>

</xml_diff>